<commit_message>
to bind optional building
</commit_message>
<xml_diff>
--- a/learningMVVM/WpfApp1/Resources/IndexChart.xlsx
+++ b/learningMVVM/WpfApp1/Resources/IndexChart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D473D2-F82A-4542-8C55-5825FC53617B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304EF370-03CE-469A-A0A1-2EF091294189}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -249,9 +249,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -542,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43016940-33EA-4FA0-BE30-386BED332A68}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -559,215 +558,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="F11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>